<commit_message>
27NOV commit, working, 2 PNs
</commit_message>
<xml_diff>
--- a/Dashboard Skeleton.xlsx
+++ b/Dashboard Skeleton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdarden\Desktop\Personal BS\ISE 535\Injection_Molding_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E142C7AA-967F-4A23-8771-A93E699033A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAD1212-C02C-4E3E-BC4A-B3AE0FD58312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{726C1940-1393-48E3-9CCB-910A532FDD8F}"/>
+    <workbookView xWindow="750" yWindow="2060" windowWidth="38150" windowHeight="13040" xr2:uid="{726C1940-1393-48E3-9CCB-910A532FDD8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,10 +57,10 @@
     <t>Yield</t>
   </si>
   <si>
-    <t>Pie Chart of Defects</t>
+    <t>Logo</t>
   </si>
   <si>
-    <t>Logo</t>
+    <t>Defect Bar Plot</t>
   </si>
 </sst>
 </file>
@@ -103,19 +103,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -125,11 +113,103 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -138,17 +218,68 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,263 +594,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB64321B-5237-4DA7-AF59-34B5E3474AEA}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="7" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="35"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="37"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="39"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="24"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="30"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="30"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="30"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="30"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="30"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="30"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="30"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="30"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="30"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="30"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="31"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I1:J3"/>
+    <mergeCell ref="K1:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>